<commit_message>
Deploying to gh-pages from  @ aa31d9f23ad775a2bdc8161c9faf363631d84bea 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_2-3-4.xlsx
+++ b/assets/excel/2021_2-3-4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B181652F-CAF5-447E-92B6-D9F4458DA2B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D205E60-2E6F-4554-B78D-45A88CC93F98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{0C07CBDE-D804-47FE-A309-854275EC75AA}"/>
   </bookViews>
@@ -176,7 +176,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="###\ ###\ ###"/>
+  </numFmts>
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,6 +355,11 @@
       <sz val="6"/>
       <color theme="10"/>
       <name val="NDSFrutiger 45 Light"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color theme="1"/>
+      <name val="NDSFrutiger 55 Roman"/>
     </font>
   </fonts>
   <fills count="33">
@@ -756,23 +764,8 @@
     <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment vertical="center"/>
@@ -797,12 +790,6 @@
     <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -811,6 +798,40 @@
     </xf>
     <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1173,7 +1194,7 @@
   <dimension ref="B1:R46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
+      <selection activeCell="C10" sqref="C10:R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,1883 +1204,1883 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
     </row>
     <row r="2" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
     </row>
     <row r="4" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
     </row>
     <row r="6" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="1"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="17"/>
     </row>
     <row r="7" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="13">
+      <c r="B7" s="14"/>
+      <c r="C7" s="8">
         <v>2005</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="8">
         <v>2006</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="8">
         <v>2007</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="8">
         <v>2008</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="8">
         <v>2009</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="8">
         <v>2010</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="8">
         <v>2011</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="8">
         <v>2012</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="8">
         <v>2013</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="8">
         <v>2014</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="8">
         <v>2015</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="8">
         <v>2016</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="8">
         <v>2017</v>
       </c>
-      <c r="P7" s="13">
+      <c r="P7" s="8">
         <v>2018</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="Q7" s="8">
         <v>2019</v>
       </c>
-      <c r="R7" s="13">
+      <c r="R7" s="8">
         <v>2020</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="1"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="17"/>
     </row>
     <row r="9" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="18">
+      <c r="B9" s="11">
         <v>1</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="11">
         <v>2</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="11">
         <v>3</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="11">
         <v>4</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="11">
         <v>5</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="11">
         <v>6</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="11">
         <v>7</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="11">
         <v>8</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="11">
         <v>9</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="11">
         <v>10</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="11">
         <v>11</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="11">
         <v>12</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="11">
         <v>13</v>
       </c>
-      <c r="O9" s="18">
+      <c r="O9" s="11">
         <v>14</v>
       </c>
-      <c r="P9" s="18">
+      <c r="P9" s="11">
         <v>15</v>
       </c>
-      <c r="Q9" s="18">
+      <c r="Q9" s="11">
         <v>16</v>
       </c>
-      <c r="R9" s="18">
+      <c r="R9" s="11">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+    <row r="10" spans="2:18" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="21">
         <v>7178</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="21">
         <v>7567</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="21">
         <v>5866</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="21">
         <v>4488</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="21">
         <v>3947</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="21">
         <v>4205</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="21">
         <v>4595</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="21">
         <v>5096</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="21">
         <v>4900</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10" s="21">
         <v>4399</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="21">
         <v>4598</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="21">
         <v>4880</v>
       </c>
-      <c r="O10" s="15">
+      <c r="O10" s="21">
         <v>5044</v>
       </c>
-      <c r="P10" s="15">
+      <c r="P10" s="21">
         <v>4743</v>
       </c>
-      <c r="Q10" s="15">
+      <c r="Q10" s="21">
         <v>6722</v>
       </c>
-      <c r="R10" s="15">
+      <c r="R10" s="21">
         <v>4041</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="22">
         <v>71</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="22">
         <v>96</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="22">
         <v>109</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="22">
         <v>98</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="22">
         <v>69</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="22">
         <v>72</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="22">
         <v>126</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="22">
         <v>344</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="22">
         <v>231</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="22">
         <v>195</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="22">
         <v>191</v>
       </c>
-      <c r="N11" s="15">
+      <c r="N11" s="22">
         <v>222</v>
       </c>
-      <c r="O11" s="15">
+      <c r="O11" s="22">
         <v>224</v>
       </c>
-      <c r="P11" s="15">
+      <c r="P11" s="22">
         <v>206</v>
       </c>
-      <c r="Q11" s="15">
+      <c r="Q11" s="22">
         <v>157</v>
       </c>
-      <c r="R11" s="15">
+      <c r="R11" s="22">
         <v>127</v>
       </c>
     </row>
     <row r="12" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="22">
         <v>71</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="22">
         <v>85</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="22">
         <v>70</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="22">
         <v>88</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="22">
         <v>53</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="22">
         <v>52</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="22">
         <v>77</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="22">
         <v>89</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="22">
         <v>114</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="22">
         <v>128</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="22">
         <v>139</v>
       </c>
-      <c r="N12" s="15">
+      <c r="N12" s="22">
         <v>160</v>
       </c>
-      <c r="O12" s="15">
+      <c r="O12" s="22">
         <v>226</v>
       </c>
-      <c r="P12" s="15">
+      <c r="P12" s="22">
         <v>199</v>
       </c>
-      <c r="Q12" s="15">
+      <c r="Q12" s="22">
         <v>170</v>
       </c>
-      <c r="R12" s="15">
+      <c r="R12" s="22">
         <v>153</v>
       </c>
     </row>
     <row r="13" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="22">
         <v>34</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="22">
         <v>170</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="22">
         <v>221</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="22">
         <v>181</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="22">
         <v>222</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="22">
         <v>216</v>
       </c>
-      <c r="M13" s="15">
+      <c r="M13" s="22">
         <v>242</v>
       </c>
-      <c r="N13" s="15">
+      <c r="N13" s="22">
         <v>215</v>
       </c>
-      <c r="O13" s="15">
+      <c r="O13" s="22">
         <v>247</v>
       </c>
-      <c r="P13" s="15">
+      <c r="P13" s="22">
         <v>217</v>
       </c>
-      <c r="Q13" s="15">
+      <c r="Q13" s="22">
         <v>188</v>
       </c>
-      <c r="R13" s="15">
+      <c r="R13" s="22">
         <v>171</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="22">
         <v>914</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="22">
         <v>864</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="22">
         <v>583</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="22">
         <v>548</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="22">
         <v>434</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="22">
         <v>422</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="22">
         <v>477</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="22">
         <v>518</v>
       </c>
-      <c r="K14" s="15">
+      <c r="K14" s="22">
         <v>655</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L14" s="22">
         <v>576</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M14" s="22">
         <v>559</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="22">
         <v>650</v>
       </c>
-      <c r="O14" s="15">
+      <c r="O14" s="22">
         <v>664</v>
       </c>
-      <c r="P14" s="15">
+      <c r="P14" s="22">
         <v>598</v>
       </c>
-      <c r="Q14" s="15">
+      <c r="Q14" s="22">
         <v>644</v>
       </c>
-      <c r="R14" s="15">
+      <c r="R14" s="22">
         <v>572</v>
       </c>
     </row>
     <row r="15" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="22">
         <v>72</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="22">
         <v>90</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="22">
         <v>209</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="22">
         <v>124</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="22">
         <v>119</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="22">
         <v>136</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="22">
         <v>132</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="22">
         <v>81</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="22">
         <v>115</v>
       </c>
-      <c r="L15" s="15">
+      <c r="L15" s="22">
         <v>113</v>
       </c>
-      <c r="M15" s="15">
+      <c r="M15" s="22">
         <v>156</v>
       </c>
-      <c r="N15" s="15">
+      <c r="N15" s="22">
         <v>193</v>
       </c>
-      <c r="O15" s="15">
+      <c r="O15" s="22">
         <v>241</v>
       </c>
-      <c r="P15" s="15">
+      <c r="P15" s="22">
         <v>239</v>
       </c>
-      <c r="Q15" s="15">
+      <c r="Q15" s="22">
         <v>337</v>
       </c>
-      <c r="R15" s="15">
+      <c r="R15" s="22">
         <v>369</v>
       </c>
     </row>
     <row r="16" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="22">
         <v>496</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="22">
         <v>475</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="22">
         <v>405</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="22">
         <v>188</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="22">
         <v>257</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="22">
         <v>304</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="22">
         <v>283</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="22">
         <v>299</v>
       </c>
-      <c r="K16" s="15">
+      <c r="K16" s="22">
         <v>245</v>
       </c>
-      <c r="L16" s="15">
+      <c r="L16" s="22">
         <v>251</v>
       </c>
-      <c r="M16" s="15">
+      <c r="M16" s="22">
         <v>168</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="22">
         <v>225</v>
       </c>
-      <c r="O16" s="15">
+      <c r="O16" s="22">
         <v>157</v>
       </c>
-      <c r="P16" s="15">
+      <c r="P16" s="22">
         <v>132</v>
       </c>
-      <c r="Q16" s="15">
+      <c r="Q16" s="22">
         <v>149</v>
       </c>
-      <c r="R16" s="15">
+      <c r="R16" s="22">
         <v>131</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="22">
         <v>1630</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="22">
         <v>1800</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="22">
         <v>1198</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="22">
         <v>540</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="22">
         <v>109</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="22">
         <v>187</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I17" s="22">
         <v>258</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="22">
         <v>225</v>
       </c>
-      <c r="K17" s="15">
+      <c r="K17" s="22">
         <v>215</v>
       </c>
-      <c r="L17" s="15">
+      <c r="L17" s="22">
         <v>174</v>
       </c>
-      <c r="M17" s="15">
+      <c r="M17" s="22">
         <v>162</v>
       </c>
-      <c r="N17" s="15">
+      <c r="N17" s="22">
         <v>214</v>
       </c>
-      <c r="O17" s="15">
+      <c r="O17" s="22">
         <v>142</v>
       </c>
-      <c r="P17" s="15">
+      <c r="P17" s="22">
         <v>254</v>
       </c>
-      <c r="Q17" s="15">
+      <c r="Q17" s="22">
         <v>275</v>
       </c>
-      <c r="R17" s="15">
+      <c r="R17" s="22">
         <v>268</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="22">
         <v>2897</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="22">
         <v>2944</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="22">
         <v>2162</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="22">
         <v>2020</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="22">
         <v>2170</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="22">
         <v>1892</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="22">
         <v>2010</v>
       </c>
-      <c r="J18" s="15">
+      <c r="J18" s="22">
         <v>2361</v>
       </c>
-      <c r="K18" s="15">
+      <c r="K18" s="22">
         <v>1864</v>
       </c>
-      <c r="L18" s="15">
+      <c r="L18" s="22">
         <v>1657</v>
       </c>
-      <c r="M18" s="15">
+      <c r="M18" s="22">
         <v>1709</v>
       </c>
-      <c r="N18" s="15">
+      <c r="N18" s="22">
         <v>1278</v>
       </c>
-      <c r="O18" s="15">
+      <c r="O18" s="22">
         <v>1208</v>
       </c>
-      <c r="P18" s="15">
+      <c r="P18" s="22">
         <v>1185</v>
       </c>
-      <c r="Q18" s="15">
+      <c r="Q18" s="22">
         <v>1331</v>
       </c>
-      <c r="R18" s="15">
+      <c r="R18" s="22">
         <v>783</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="22">
         <v>322</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="22">
         <v>492</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="22">
         <v>493</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="22">
         <v>185</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="22">
         <v>143</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="22">
         <v>268</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I19" s="22">
         <v>380</v>
       </c>
-      <c r="J19" s="15">
+      <c r="J19" s="22">
         <v>325</v>
       </c>
-      <c r="K19" s="15">
+      <c r="K19" s="22">
         <v>382</v>
       </c>
-      <c r="L19" s="15">
+      <c r="L19" s="22">
         <v>148</v>
       </c>
-      <c r="M19" s="15">
+      <c r="M19" s="22">
         <v>328</v>
       </c>
-      <c r="N19" s="15">
+      <c r="N19" s="22">
         <v>449</v>
       </c>
-      <c r="O19" s="15">
+      <c r="O19" s="22">
         <v>238</v>
       </c>
-      <c r="P19" s="15">
+      <c r="P19" s="22">
         <v>180</v>
       </c>
-      <c r="Q19" s="15">
+      <c r="Q19" s="22">
         <v>303</v>
       </c>
-      <c r="R19" s="15">
+      <c r="R19" s="22">
         <v>164</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="22">
         <v>50</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="22">
         <v>41</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="22">
         <v>36</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="22">
         <v>39</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="22">
         <v>24</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="22">
         <v>21</v>
       </c>
-      <c r="I20" s="15">
+      <c r="I20" s="22">
         <v>28</v>
       </c>
-      <c r="J20" s="15">
+      <c r="J20" s="22">
         <v>20</v>
       </c>
-      <c r="K20" s="15">
+      <c r="K20" s="22">
         <v>55</v>
       </c>
-      <c r="L20" s="15">
+      <c r="L20" s="22">
         <v>64</v>
       </c>
-      <c r="M20" s="15">
+      <c r="M20" s="22">
         <v>63</v>
       </c>
-      <c r="N20" s="15">
+      <c r="N20" s="22">
         <v>295</v>
       </c>
-      <c r="O20" s="15">
+      <c r="O20" s="22">
         <v>672</v>
       </c>
-      <c r="P20" s="15">
+      <c r="P20" s="22">
         <v>582</v>
       </c>
-      <c r="Q20" s="15">
+      <c r="Q20" s="22">
         <v>2217</v>
       </c>
-      <c r="R20" s="15">
+      <c r="R20" s="22">
         <v>441</v>
       </c>
     </row>
-    <row r="21" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="14" t="s">
+    <row r="21" spans="2:18" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="21">
         <v>1533</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="21">
         <v>1534</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="21">
         <v>1289</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="21">
         <v>1232</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="21">
         <v>1017</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="21">
         <v>1165</v>
       </c>
-      <c r="I21" s="15">
+      <c r="I21" s="21">
         <v>1263</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="21">
         <v>1482</v>
       </c>
-      <c r="K21" s="15">
+      <c r="K21" s="21">
         <v>1739</v>
       </c>
-      <c r="L21" s="15">
+      <c r="L21" s="21">
         <v>1769</v>
       </c>
-      <c r="M21" s="15">
+      <c r="M21" s="21">
         <v>1765</v>
       </c>
-      <c r="N21" s="15">
+      <c r="N21" s="21">
         <v>2262</v>
       </c>
-      <c r="O21" s="15">
+      <c r="O21" s="21">
         <v>2787</v>
       </c>
-      <c r="P21" s="15">
+      <c r="P21" s="21">
         <v>2501</v>
       </c>
-      <c r="Q21" s="15">
+      <c r="Q21" s="21">
         <v>4241</v>
       </c>
-      <c r="R21" s="15">
+      <c r="R21" s="21">
         <v>2376</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="22">
         <v>568</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="22">
         <v>525</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="22">
         <v>521</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="22">
         <v>564</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="22">
         <v>542</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="22">
         <v>489</v>
       </c>
-      <c r="I22" s="15">
+      <c r="I22" s="22">
         <v>599</v>
       </c>
-      <c r="J22" s="15">
+      <c r="J22" s="22">
         <v>596</v>
       </c>
-      <c r="K22" s="15">
+      <c r="K22" s="22">
         <v>589</v>
       </c>
-      <c r="L22" s="15">
+      <c r="L22" s="22">
         <v>596</v>
       </c>
-      <c r="M22" s="15">
+      <c r="M22" s="22">
         <v>625</v>
       </c>
-      <c r="N22" s="15">
+      <c r="N22" s="22">
         <v>647</v>
       </c>
-      <c r="O22" s="15">
+      <c r="O22" s="22">
         <v>673</v>
       </c>
-      <c r="P22" s="15">
+      <c r="P22" s="22">
         <v>658</v>
       </c>
-      <c r="Q22" s="15">
+      <c r="Q22" s="22">
         <v>661</v>
       </c>
-      <c r="R22" s="15">
+      <c r="R22" s="22">
         <v>744</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="22">
         <v>111</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="22">
         <v>81</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="22">
         <v>112</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="22">
         <v>76</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G23" s="22">
         <v>73</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="22">
         <v>89</v>
       </c>
-      <c r="I23" s="15">
+      <c r="I23" s="22">
         <v>96</v>
       </c>
-      <c r="J23" s="15">
+      <c r="J23" s="22">
         <v>110</v>
       </c>
-      <c r="K23" s="15">
+      <c r="K23" s="22">
         <v>111</v>
       </c>
-      <c r="L23" s="15">
+      <c r="L23" s="22">
         <v>119</v>
       </c>
-      <c r="M23" s="15">
+      <c r="M23" s="22">
         <v>112</v>
       </c>
-      <c r="N23" s="15">
+      <c r="N23" s="22">
         <v>134</v>
       </c>
-      <c r="O23" s="15">
+      <c r="O23" s="22">
         <v>108</v>
       </c>
-      <c r="P23" s="15">
+      <c r="P23" s="22">
         <v>119</v>
       </c>
-      <c r="Q23" s="15">
+      <c r="Q23" s="22">
         <v>124</v>
       </c>
-      <c r="R23" s="15">
+      <c r="R23" s="22">
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
+    <row r="24" spans="2:18" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="21">
         <v>213</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="21">
         <v>250</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="21">
         <v>266</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="21">
         <v>233</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="21">
         <v>211</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="21">
         <v>225</v>
       </c>
-      <c r="I24" s="15">
+      <c r="I24" s="21">
         <v>211</v>
       </c>
-      <c r="J24" s="15">
+      <c r="J24" s="21">
         <v>211</v>
       </c>
-      <c r="K24" s="15">
+      <c r="K24" s="21">
         <v>228</v>
       </c>
-      <c r="L24" s="15">
+      <c r="L24" s="21">
         <v>256</v>
       </c>
-      <c r="M24" s="15">
+      <c r="M24" s="21">
         <v>260</v>
       </c>
-      <c r="N24" s="15">
+      <c r="N24" s="21">
         <v>270</v>
       </c>
-      <c r="O24" s="15">
+      <c r="O24" s="21">
         <v>296</v>
       </c>
-      <c r="P24" s="15">
+      <c r="P24" s="21">
         <v>247</v>
       </c>
-      <c r="Q24" s="15">
+      <c r="Q24" s="21">
         <v>288</v>
       </c>
-      <c r="R24" s="15">
+      <c r="R24" s="21">
         <v>272</v>
       </c>
     </row>
-    <row r="25" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+    <row r="25" spans="2:18" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="21">
         <v>2704</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="21">
         <v>2851</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="21">
         <v>2375</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="21">
         <v>2272</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="21">
         <v>2338</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="21">
         <v>2290</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="21">
         <v>2443</v>
       </c>
-      <c r="J25" s="15">
+      <c r="J25" s="21">
         <v>2488</v>
       </c>
-      <c r="K25" s="15">
+      <c r="K25" s="21">
         <v>2348</v>
       </c>
-      <c r="L25" s="15">
+      <c r="L25" s="21">
         <v>2364</v>
       </c>
-      <c r="M25" s="15">
+      <c r="M25" s="21">
         <v>2392</v>
       </c>
-      <c r="N25" s="15">
+      <c r="N25" s="21">
         <v>2614</v>
       </c>
-      <c r="O25" s="15">
+      <c r="O25" s="21">
         <v>2599</v>
       </c>
-      <c r="P25" s="15">
+      <c r="P25" s="21">
         <v>2694</v>
       </c>
-      <c r="Q25" s="15">
+      <c r="Q25" s="21">
         <v>3120</v>
       </c>
-      <c r="R25" s="15">
+      <c r="R25" s="21">
         <v>3645</v>
       </c>
     </row>
     <row r="26" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="22">
         <v>236</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="22">
         <v>227</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="22">
         <v>230</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="22">
         <v>219</v>
       </c>
-      <c r="G26" s="15">
+      <c r="G26" s="22">
         <v>210</v>
       </c>
-      <c r="H26" s="15">
+      <c r="H26" s="22">
         <v>161</v>
       </c>
-      <c r="I26" s="15">
+      <c r="I26" s="22">
         <v>124</v>
       </c>
-      <c r="J26" s="15">
+      <c r="J26" s="22">
         <v>121</v>
       </c>
-      <c r="K26" s="15">
+      <c r="K26" s="22">
         <v>129</v>
       </c>
-      <c r="L26" s="15">
+      <c r="L26" s="22">
         <v>129</v>
       </c>
-      <c r="M26" s="15">
+      <c r="M26" s="22">
         <v>129</v>
       </c>
-      <c r="N26" s="15">
+      <c r="N26" s="22">
         <v>150</v>
       </c>
-      <c r="O26" s="15">
+      <c r="O26" s="22">
         <v>158</v>
       </c>
-      <c r="P26" s="15">
+      <c r="P26" s="22">
         <v>131</v>
       </c>
-      <c r="Q26" s="15">
+      <c r="Q26" s="22">
         <v>167</v>
       </c>
-      <c r="R26" s="15">
+      <c r="R26" s="22">
         <v>184</v>
       </c>
     </row>
     <row r="27" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="22">
         <v>395</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="22">
         <v>454</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="22">
         <v>377</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="22">
         <v>367</v>
       </c>
-      <c r="G27" s="15">
+      <c r="G27" s="22">
         <v>335</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27" s="22">
         <v>295</v>
       </c>
-      <c r="I27" s="15">
+      <c r="I27" s="22">
         <v>240</v>
       </c>
-      <c r="J27" s="15">
+      <c r="J27" s="22">
         <v>209</v>
       </c>
-      <c r="K27" s="15">
+      <c r="K27" s="22">
         <v>243</v>
       </c>
-      <c r="L27" s="15">
+      <c r="L27" s="22">
         <v>254</v>
       </c>
-      <c r="M27" s="15">
+      <c r="M27" s="22">
         <v>259</v>
       </c>
-      <c r="N27" s="15">
+      <c r="N27" s="22">
         <v>303</v>
       </c>
-      <c r="O27" s="15">
+      <c r="O27" s="22">
         <v>238</v>
       </c>
-      <c r="P27" s="15">
+      <c r="P27" s="22">
         <v>233</v>
       </c>
-      <c r="Q27" s="15">
+      <c r="Q27" s="22">
         <v>209</v>
       </c>
-      <c r="R27" s="15">
+      <c r="R27" s="22">
         <v>194</v>
       </c>
     </row>
     <row r="28" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="22">
         <v>52</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="22">
         <v>44</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="22">
         <v>33</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="22">
         <v>38</v>
       </c>
-      <c r="G28" s="15">
+      <c r="G28" s="22">
         <v>34</v>
       </c>
-      <c r="H28" s="15">
+      <c r="H28" s="22">
         <v>41</v>
       </c>
-      <c r="I28" s="15">
+      <c r="I28" s="22">
         <v>44</v>
       </c>
-      <c r="J28" s="15">
+      <c r="J28" s="22">
         <v>64</v>
       </c>
-      <c r="K28" s="15">
+      <c r="K28" s="22">
         <v>61</v>
       </c>
-      <c r="L28" s="15">
+      <c r="L28" s="22">
         <v>63</v>
       </c>
-      <c r="M28" s="15">
+      <c r="M28" s="22">
         <v>65</v>
       </c>
-      <c r="N28" s="15">
+      <c r="N28" s="22">
         <v>96</v>
       </c>
-      <c r="O28" s="15">
+      <c r="O28" s="22">
         <v>103</v>
       </c>
-      <c r="P28" s="15">
+      <c r="P28" s="22">
         <v>73</v>
       </c>
-      <c r="Q28" s="15">
+      <c r="Q28" s="22">
         <v>157</v>
       </c>
-      <c r="R28" s="15">
+      <c r="R28" s="22">
         <v>117</v>
       </c>
     </row>
     <row r="29" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="22">
         <v>516</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="22">
         <v>251</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="22">
         <v>286</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="22">
         <v>306</v>
       </c>
-      <c r="G29" s="15">
+      <c r="G29" s="22">
         <v>361</v>
       </c>
-      <c r="H29" s="15">
+      <c r="H29" s="22">
         <v>392</v>
       </c>
-      <c r="I29" s="15">
+      <c r="I29" s="22">
         <v>434</v>
       </c>
-      <c r="J29" s="15">
+      <c r="J29" s="22">
         <v>273</v>
       </c>
-      <c r="K29" s="15">
+      <c r="K29" s="22">
         <v>326</v>
       </c>
-      <c r="L29" s="15">
+      <c r="L29" s="22">
         <v>317</v>
       </c>
-      <c r="M29" s="15">
+      <c r="M29" s="22">
         <v>313</v>
       </c>
-      <c r="N29" s="15">
+      <c r="N29" s="22">
         <v>430</v>
       </c>
-      <c r="O29" s="15">
+      <c r="O29" s="22">
         <v>403</v>
       </c>
-      <c r="P29" s="15">
+      <c r="P29" s="22">
         <v>389</v>
       </c>
-      <c r="Q29" s="15">
+      <c r="Q29" s="22">
         <v>465</v>
       </c>
-      <c r="R29" s="15">
+      <c r="R29" s="22">
         <v>477</v>
       </c>
     </row>
     <row r="30" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="22">
         <v>348</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="22">
         <v>386</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="22">
         <v>362</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="22">
         <v>303</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G30" s="22">
         <v>323</v>
       </c>
-      <c r="H30" s="15">
+      <c r="H30" s="22">
         <v>245</v>
       </c>
-      <c r="I30" s="15">
+      <c r="I30" s="22">
         <v>255</v>
       </c>
-      <c r="J30" s="15">
+      <c r="J30" s="22">
         <v>227</v>
       </c>
-      <c r="K30" s="15">
+      <c r="K30" s="22">
         <v>227</v>
       </c>
-      <c r="L30" s="15">
+      <c r="L30" s="22">
         <v>262</v>
       </c>
-      <c r="M30" s="15">
+      <c r="M30" s="22">
         <v>221</v>
       </c>
-      <c r="N30" s="15">
+      <c r="N30" s="22">
         <v>255</v>
       </c>
-      <c r="O30" s="15">
+      <c r="O30" s="22">
         <v>260</v>
       </c>
-      <c r="P30" s="15">
+      <c r="P30" s="22">
         <v>243</v>
       </c>
-      <c r="Q30" s="15">
+      <c r="Q30" s="22">
         <v>308</v>
       </c>
-      <c r="R30" s="15">
+      <c r="R30" s="22">
         <v>336</v>
       </c>
     </row>
     <row r="31" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="22">
         <v>87</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="22">
         <v>76</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="22">
         <v>46</v>
       </c>
-      <c r="F31" s="15">
+      <c r="F31" s="22">
         <v>52</v>
       </c>
-      <c r="G31" s="15">
+      <c r="G31" s="22">
         <v>67</v>
       </c>
-      <c r="H31" s="15">
+      <c r="H31" s="22">
         <v>33</v>
       </c>
-      <c r="I31" s="15">
+      <c r="I31" s="22">
         <v>47</v>
       </c>
-      <c r="J31" s="15">
+      <c r="J31" s="22">
         <v>49</v>
       </c>
-      <c r="K31" s="15">
+      <c r="K31" s="22">
         <v>40</v>
       </c>
-      <c r="L31" s="15">
+      <c r="L31" s="22">
         <v>61</v>
       </c>
-      <c r="M31" s="15">
+      <c r="M31" s="22">
         <v>66</v>
       </c>
-      <c r="N31" s="15">
+      <c r="N31" s="22">
         <v>77</v>
       </c>
-      <c r="O31" s="15">
+      <c r="O31" s="22">
         <v>60</v>
       </c>
-      <c r="P31" s="15">
+      <c r="P31" s="22">
         <v>57</v>
       </c>
-      <c r="Q31" s="15">
+      <c r="Q31" s="22">
         <v>77</v>
       </c>
-      <c r="R31" s="15">
+      <c r="R31" s="22">
         <v>120</v>
       </c>
     </row>
     <row r="32" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="22">
         <v>171</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="22">
         <v>183</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="22">
         <v>210</v>
       </c>
-      <c r="F32" s="15">
+      <c r="F32" s="22">
         <v>208</v>
       </c>
-      <c r="G32" s="15">
+      <c r="G32" s="22">
         <v>225</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="22">
         <v>219</v>
       </c>
-      <c r="I32" s="15">
+      <c r="I32" s="22">
         <v>219</v>
       </c>
-      <c r="J32" s="15">
+      <c r="J32" s="22">
         <v>208</v>
       </c>
-      <c r="K32" s="15">
+      <c r="K32" s="22">
         <v>247</v>
       </c>
-      <c r="L32" s="15">
+      <c r="L32" s="22">
         <v>300</v>
       </c>
-      <c r="M32" s="15">
+      <c r="M32" s="22">
         <v>398</v>
       </c>
-      <c r="N32" s="15">
+      <c r="N32" s="22">
         <v>368</v>
       </c>
-      <c r="O32" s="15">
+      <c r="O32" s="22">
         <v>444</v>
       </c>
-      <c r="P32" s="15">
+      <c r="P32" s="22">
         <v>664</v>
       </c>
-      <c r="Q32" s="15">
+      <c r="Q32" s="22">
         <v>857</v>
       </c>
-      <c r="R32" s="15">
+      <c r="R32" s="22">
         <v>1414</v>
       </c>
     </row>
     <row r="33" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="22">
         <v>137</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="22">
         <v>160</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="22">
         <v>158</v>
       </c>
-      <c r="F33" s="15">
+      <c r="F33" s="22">
         <v>110</v>
       </c>
-      <c r="G33" s="15">
+      <c r="G33" s="22">
         <v>227</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33" s="22">
         <v>280</v>
       </c>
-      <c r="I33" s="15">
+      <c r="I33" s="22">
         <v>419</v>
       </c>
-      <c r="J33" s="15">
+      <c r="J33" s="22">
         <v>667</v>
       </c>
-      <c r="K33" s="15">
+      <c r="K33" s="22">
         <v>387</v>
       </c>
-      <c r="L33" s="15">
+      <c r="L33" s="22">
         <v>277</v>
       </c>
-      <c r="M33" s="15">
+      <c r="M33" s="22">
         <v>266</v>
       </c>
-      <c r="N33" s="15">
+      <c r="N33" s="22">
         <v>265</v>
       </c>
-      <c r="O33" s="15">
+      <c r="O33" s="22">
         <v>259</v>
       </c>
-      <c r="P33" s="15">
+      <c r="P33" s="22">
         <v>290</v>
       </c>
-      <c r="Q33" s="15">
+      <c r="Q33" s="22">
         <v>224</v>
       </c>
-      <c r="R33" s="15">
+      <c r="R33" s="22">
         <v>199</v>
       </c>
     </row>
     <row r="34" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C34" s="22">
         <v>1</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="22">
         <v>2</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="22">
         <v>1</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F34" s="22">
         <v>0</v>
       </c>
-      <c r="G34" s="15">
+      <c r="G34" s="22">
         <v>1</v>
       </c>
-      <c r="H34" s="15">
+      <c r="H34" s="22">
         <v>2</v>
       </c>
-      <c r="I34" s="15">
+      <c r="I34" s="22">
         <v>3</v>
       </c>
-      <c r="J34" s="15">
+      <c r="J34" s="22">
         <v>2</v>
       </c>
-      <c r="K34" s="15">
+      <c r="K34" s="22">
         <v>1</v>
       </c>
-      <c r="L34" s="15">
+      <c r="L34" s="22">
         <v>0</v>
       </c>
-      <c r="M34" s="15">
+      <c r="M34" s="22">
         <v>1</v>
       </c>
-      <c r="N34" s="15">
+      <c r="N34" s="22">
         <v>0</v>
       </c>
-      <c r="O34" s="15">
+      <c r="O34" s="22">
         <v>2</v>
       </c>
-      <c r="P34" s="15">
+      <c r="P34" s="22">
         <v>1</v>
       </c>
-      <c r="Q34" s="15">
+      <c r="Q34" s="22">
         <v>3</v>
       </c>
-      <c r="R34" s="15">
+      <c r="R34" s="22">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C35" s="22">
         <v>222</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="22">
         <v>246</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="22">
         <v>222</v>
       </c>
-      <c r="F35" s="15">
+      <c r="F35" s="22">
         <v>147</v>
       </c>
-      <c r="G35" s="15">
+      <c r="G35" s="22">
         <v>184</v>
       </c>
-      <c r="H35" s="15">
+      <c r="H35" s="22">
         <v>152</v>
       </c>
-      <c r="I35" s="15">
+      <c r="I35" s="22">
         <v>144</v>
       </c>
-      <c r="J35" s="15">
+      <c r="J35" s="22">
         <v>133</v>
       </c>
-      <c r="K35" s="15">
+      <c r="K35" s="22">
         <v>150</v>
       </c>
-      <c r="L35" s="15">
+      <c r="L35" s="22">
         <v>107</v>
       </c>
-      <c r="M35" s="15">
+      <c r="M35" s="22">
         <v>112</v>
       </c>
-      <c r="N35" s="15">
+      <c r="N35" s="22">
         <v>108</v>
       </c>
-      <c r="O35" s="15">
+      <c r="O35" s="22">
         <v>171</v>
       </c>
-      <c r="P35" s="15">
+      <c r="P35" s="22">
         <v>127</v>
       </c>
-      <c r="Q35" s="15">
+      <c r="Q35" s="22">
         <v>137</v>
       </c>
-      <c r="R35" s="15">
+      <c r="R35" s="22">
         <v>171</v>
       </c>
     </row>
     <row r="36" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="15">
+      <c r="C36" s="22">
         <v>150</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="22">
         <v>171</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="22">
         <v>136</v>
       </c>
-      <c r="F36" s="15">
+      <c r="F36" s="22">
         <v>99</v>
       </c>
-      <c r="G36" s="15">
+      <c r="G36" s="22">
         <v>125</v>
       </c>
-      <c r="H36" s="15">
+      <c r="H36" s="22">
         <v>125</v>
       </c>
-      <c r="I36" s="15">
+      <c r="I36" s="22">
         <v>99</v>
       </c>
-      <c r="J36" s="15">
+      <c r="J36" s="22">
         <v>117</v>
       </c>
-      <c r="K36" s="15">
+      <c r="K36" s="22">
         <v>113</v>
       </c>
-      <c r="L36" s="15">
+      <c r="L36" s="22">
         <v>83</v>
       </c>
-      <c r="M36" s="15">
+      <c r="M36" s="22">
         <v>80</v>
       </c>
-      <c r="N36" s="15">
+      <c r="N36" s="22">
         <v>70</v>
       </c>
-      <c r="O36" s="15">
+      <c r="O36" s="22">
         <v>138</v>
       </c>
-      <c r="P36" s="15">
+      <c r="P36" s="22">
         <v>104</v>
       </c>
-      <c r="Q36" s="15">
+      <c r="Q36" s="22">
         <v>115</v>
       </c>
-      <c r="R36" s="15">
+      <c r="R36" s="22">
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="17" t="s">
+    <row r="37" spans="2:18" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C37" s="24">
         <v>10886</v>
       </c>
-      <c r="D37" s="16">
+      <c r="D37" s="24">
         <v>11441</v>
       </c>
-      <c r="E37" s="16">
+      <c r="E37" s="24">
         <v>9251</v>
       </c>
-      <c r="F37" s="16">
+      <c r="F37" s="24">
         <v>7704</v>
       </c>
-      <c r="G37" s="16">
+      <c r="G37" s="24">
         <v>7223</v>
       </c>
-      <c r="H37" s="16">
+      <c r="H37" s="24">
         <v>7363</v>
       </c>
-      <c r="I37" s="16">
+      <c r="I37" s="24">
         <v>7995</v>
       </c>
-      <c r="J37" s="16">
+      <c r="J37" s="24">
         <v>8526</v>
       </c>
-      <c r="K37" s="16">
+      <c r="K37" s="24">
         <v>8216</v>
       </c>
-      <c r="L37" s="16">
+      <c r="L37" s="24">
         <v>7722</v>
       </c>
-      <c r="M37" s="16">
+      <c r="M37" s="24">
         <v>7988</v>
       </c>
-      <c r="N37" s="16">
+      <c r="N37" s="24">
         <v>8519</v>
       </c>
-      <c r="O37" s="16">
+      <c r="O37" s="24">
         <v>8785</v>
       </c>
-      <c r="P37" s="16">
+      <c r="P37" s="24">
         <v>8470</v>
       </c>
-      <c r="Q37" s="16">
+      <c r="Q37" s="24">
         <v>10932</v>
       </c>
-      <c r="R37" s="16">
+      <c r="R37" s="24">
         <v>8878</v>
       </c>
     </row>
     <row r="38" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="8"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="3"/>
     </row>
     <row r="39" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="8"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="3"/>
     </row>
     <row r="40" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="17"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
-      <c r="Q40" s="7"/>
-      <c r="R40" s="7"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
     </row>
     <row r="41" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="7"/>
-      <c r="P41" s="7"/>
-      <c r="Q41" s="7"/>
-      <c r="R41" s="7"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
     </row>
     <row r="42" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="17"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="7"/>
-      <c r="Q42" s="7"/>
-      <c r="R42" s="7"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
     </row>
     <row r="43" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="7"/>
-      <c r="P43" s="7"/>
-      <c r="Q43" s="7"/>
-      <c r="R43" s="7"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
     </row>
     <row r="44" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="7"/>
-      <c r="P44" s="7"/>
-      <c r="Q44" s="7"/>
-      <c r="R44" s="7"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
     </row>
     <row r="45" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7"/>
-      <c r="O45" s="7"/>
-      <c r="P45" s="7"/>
-      <c r="Q45" s="7"/>
-      <c r="R45" s="7"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
     </row>
     <row r="46" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7"/>
-      <c r="P46" s="7"/>
-      <c r="Q46" s="7"/>
-      <c r="R46" s="7"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ bb9e081d4f3078a35e8b4c5b9e20cf673bde1aec 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_2-3-4.xlsx
+++ b/assets/excel/2021_2-3-4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D205E60-2E6F-4554-B78D-45A88CC93F98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E159341-5232-49C3-B2AC-874D2705D36C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{0C07CBDE-D804-47FE-A309-854275EC75AA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
   </si>
@@ -86,9 +86,6 @@
     <t xml:space="preserve">  Ukraine                   </t>
   </si>
   <si>
-    <t xml:space="preserve">  Vereinigtes Königreich GB, Nordirland</t>
-  </si>
-  <si>
     <t xml:space="preserve"> EU Staaten                 </t>
   </si>
   <si>
@@ -171,6 +168,23 @@
       <t>1)</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  Vereinigtes Königreich GB, Nordirland</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="NDSFrutiger 45 Light"/>
+      </rPr>
+      <t>2)</t>
+    </r>
+  </si>
+  <si>
+    <t>2) einschließlich Brittisch abhängiger Gebiete</t>
+  </si>
 </sst>
 </file>
 
@@ -179,7 +193,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###\ ###\ ###"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,6 +374,12 @@
       <sz val="6"/>
       <color theme="1"/>
       <name val="NDSFrutiger 55 Roman"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="6"/>
+      <color theme="1"/>
+      <name val="NDSFrutiger 45 Light"/>
     </font>
   </fonts>
   <fills count="33">
@@ -799,21 +819,6 @@
     <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -832,6 +837,21 @@
     </xf>
     <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1191,10 +1211,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7E64D10-9C9A-44E2-8806-D26C8D26226A}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="B1:R46"/>
+  <dimension ref="B1:R47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:R37"/>
+      <selection activeCell="B6" sqref="B6:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,30 +1288,30 @@
       <c r="R4" s="1"/>
     </row>
     <row r="6" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="17"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="24"/>
     </row>
     <row r="7" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="8">
         <v>2005</v>
       </c>
@@ -1342,25 +1362,25 @@
       </c>
     </row>
     <row r="8" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
-      <c r="C8" s="16" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="17"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="24"/>
     </row>
     <row r="9" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
@@ -1415,56 +1435,56 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:18" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="19" t="s">
+    <row r="10" spans="2:18" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="16">
         <v>7178</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="16">
         <v>7567</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="16">
         <v>5866</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="16">
         <v>4488</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="16">
         <v>3947</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="16">
         <v>4205</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="16">
         <v>4595</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="16">
         <v>5096</v>
       </c>
-      <c r="K10" s="21">
+      <c r="K10" s="16">
         <v>4900</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="16">
         <v>4399</v>
       </c>
-      <c r="M10" s="21">
+      <c r="M10" s="16">
         <v>4598</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="16">
         <v>4880</v>
       </c>
-      <c r="O10" s="21">
+      <c r="O10" s="16">
         <v>5044</v>
       </c>
-      <c r="P10" s="21">
+      <c r="P10" s="16">
         <v>4743</v>
       </c>
-      <c r="Q10" s="21">
+      <c r="Q10" s="16">
         <v>6722</v>
       </c>
-      <c r="R10" s="21">
+      <c r="R10" s="16">
         <v>4041</v>
       </c>
     </row>
@@ -1472,52 +1492,52 @@
       <c r="B11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="17">
         <v>71</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="17">
         <v>96</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="17">
         <v>109</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="17">
         <v>98</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="17">
         <v>69</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="17">
         <v>72</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="17">
         <v>126</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="17">
         <v>344</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="17">
         <v>231</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="17">
         <v>195</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="17">
         <v>191</v>
       </c>
-      <c r="N11" s="22">
+      <c r="N11" s="17">
         <v>222</v>
       </c>
-      <c r="O11" s="22">
+      <c r="O11" s="17">
         <v>224</v>
       </c>
-      <c r="P11" s="22">
+      <c r="P11" s="17">
         <v>206</v>
       </c>
-      <c r="Q11" s="22">
+      <c r="Q11" s="17">
         <v>157</v>
       </c>
-      <c r="R11" s="22">
+      <c r="R11" s="17">
         <v>127</v>
       </c>
     </row>
@@ -1525,52 +1545,52 @@
       <c r="B12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="17">
         <v>71</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="17">
         <v>85</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="17">
         <v>70</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="17">
         <v>88</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="17">
         <v>53</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="17">
         <v>52</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="17">
         <v>77</v>
       </c>
-      <c r="J12" s="22">
+      <c r="J12" s="17">
         <v>89</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="17">
         <v>114</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="17">
         <v>128</v>
       </c>
-      <c r="M12" s="22">
+      <c r="M12" s="17">
         <v>139</v>
       </c>
-      <c r="N12" s="22">
+      <c r="N12" s="17">
         <v>160</v>
       </c>
-      <c r="O12" s="22">
+      <c r="O12" s="17">
         <v>226</v>
       </c>
-      <c r="P12" s="22">
+      <c r="P12" s="17">
         <v>199</v>
       </c>
-      <c r="Q12" s="22">
+      <c r="Q12" s="17">
         <v>170</v>
       </c>
-      <c r="R12" s="22">
+      <c r="R12" s="17">
         <v>153</v>
       </c>
     </row>
@@ -1578,52 +1598,52 @@
       <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="17">
         <v>34</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="17">
         <v>170</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="17">
         <v>221</v>
       </c>
-      <c r="J13" s="22">
+      <c r="J13" s="17">
         <v>181</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="17">
         <v>222</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="17">
         <v>216</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="17">
         <v>242</v>
       </c>
-      <c r="N13" s="22">
+      <c r="N13" s="17">
         <v>215</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="17">
         <v>247</v>
       </c>
-      <c r="P13" s="22">
+      <c r="P13" s="17">
         <v>217</v>
       </c>
-      <c r="Q13" s="22">
+      <c r="Q13" s="17">
         <v>188</v>
       </c>
-      <c r="R13" s="22">
+      <c r="R13" s="17">
         <v>171</v>
       </c>
     </row>
@@ -1631,52 +1651,52 @@
       <c r="B14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="17">
         <v>914</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="17">
         <v>864</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="17">
         <v>583</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="17">
         <v>548</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="17">
         <v>434</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="17">
         <v>422</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="17">
         <v>477</v>
       </c>
-      <c r="J14" s="22">
+      <c r="J14" s="17">
         <v>518</v>
       </c>
-      <c r="K14" s="22">
+      <c r="K14" s="17">
         <v>655</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="17">
         <v>576</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="17">
         <v>559</v>
       </c>
-      <c r="N14" s="22">
+      <c r="N14" s="17">
         <v>650</v>
       </c>
-      <c r="O14" s="22">
+      <c r="O14" s="17">
         <v>664</v>
       </c>
-      <c r="P14" s="22">
+      <c r="P14" s="17">
         <v>598</v>
       </c>
-      <c r="Q14" s="22">
+      <c r="Q14" s="17">
         <v>644</v>
       </c>
-      <c r="R14" s="22">
+      <c r="R14" s="17">
         <v>572</v>
       </c>
     </row>
@@ -1684,52 +1704,52 @@
       <c r="B15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="17">
         <v>72</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="17">
         <v>90</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="17">
         <v>209</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="17">
         <v>124</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="17">
         <v>119</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="17">
         <v>136</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="17">
         <v>132</v>
       </c>
-      <c r="J15" s="22">
+      <c r="J15" s="17">
         <v>81</v>
       </c>
-      <c r="K15" s="22">
+      <c r="K15" s="17">
         <v>115</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="17">
         <v>113</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="17">
         <v>156</v>
       </c>
-      <c r="N15" s="22">
+      <c r="N15" s="17">
         <v>193</v>
       </c>
-      <c r="O15" s="22">
+      <c r="O15" s="17">
         <v>241</v>
       </c>
-      <c r="P15" s="22">
+      <c r="P15" s="17">
         <v>239</v>
       </c>
-      <c r="Q15" s="22">
+      <c r="Q15" s="17">
         <v>337</v>
       </c>
-      <c r="R15" s="22">
+      <c r="R15" s="17">
         <v>369</v>
       </c>
     </row>
@@ -1737,105 +1757,105 @@
       <c r="B16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="17">
         <v>496</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="17">
         <v>475</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="17">
         <v>405</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="17">
         <v>188</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="17">
         <v>257</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="17">
         <v>304</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="17">
         <v>283</v>
       </c>
-      <c r="J16" s="22">
+      <c r="J16" s="17">
         <v>299</v>
       </c>
-      <c r="K16" s="22">
+      <c r="K16" s="17">
         <v>245</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="17">
         <v>251</v>
       </c>
-      <c r="M16" s="22">
+      <c r="M16" s="17">
         <v>168</v>
       </c>
-      <c r="N16" s="22">
+      <c r="N16" s="17">
         <v>225</v>
       </c>
-      <c r="O16" s="22">
+      <c r="O16" s="17">
         <v>157</v>
       </c>
-      <c r="P16" s="22">
+      <c r="P16" s="17">
         <v>132</v>
       </c>
-      <c r="Q16" s="22">
+      <c r="Q16" s="17">
         <v>149</v>
       </c>
-      <c r="R16" s="22">
+      <c r="R16" s="17">
         <v>131</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="22">
+        <v>39</v>
+      </c>
+      <c r="C17" s="17">
         <v>1630</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="17">
         <v>1800</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="17">
         <v>1198</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="17">
         <v>540</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="17">
         <v>109</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="17">
         <v>187</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I17" s="17">
         <v>258</v>
       </c>
-      <c r="J17" s="22">
+      <c r="J17" s="17">
         <v>225</v>
       </c>
-      <c r="K17" s="22">
+      <c r="K17" s="17">
         <v>215</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="17">
         <v>174</v>
       </c>
-      <c r="M17" s="22">
+      <c r="M17" s="17">
         <v>162</v>
       </c>
-      <c r="N17" s="22">
+      <c r="N17" s="17">
         <v>214</v>
       </c>
-      <c r="O17" s="22">
+      <c r="O17" s="17">
         <v>142</v>
       </c>
-      <c r="P17" s="22">
+      <c r="P17" s="17">
         <v>254</v>
       </c>
-      <c r="Q17" s="22">
+      <c r="Q17" s="17">
         <v>275</v>
       </c>
-      <c r="R17" s="22">
+      <c r="R17" s="17">
         <v>268</v>
       </c>
     </row>
@@ -1843,52 +1863,52 @@
       <c r="B18" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="17">
         <v>2897</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="17">
         <v>2944</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="17">
         <v>2162</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="17">
         <v>2020</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="17">
         <v>2170</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="17">
         <v>1892</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="17">
         <v>2010</v>
       </c>
-      <c r="J18" s="22">
+      <c r="J18" s="17">
         <v>2361</v>
       </c>
-      <c r="K18" s="22">
+      <c r="K18" s="17">
         <v>1864</v>
       </c>
-      <c r="L18" s="22">
+      <c r="L18" s="17">
         <v>1657</v>
       </c>
-      <c r="M18" s="22">
+      <c r="M18" s="17">
         <v>1709</v>
       </c>
-      <c r="N18" s="22">
+      <c r="N18" s="17">
         <v>1278</v>
       </c>
-      <c r="O18" s="22">
+      <c r="O18" s="17">
         <v>1208</v>
       </c>
-      <c r="P18" s="22">
+      <c r="P18" s="17">
         <v>1185</v>
       </c>
-      <c r="Q18" s="22">
+      <c r="Q18" s="17">
         <v>1331</v>
       </c>
-      <c r="R18" s="22">
+      <c r="R18" s="17">
         <v>783</v>
       </c>
     </row>
@@ -1896,1006 +1916,1006 @@
       <c r="B19" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="17">
         <v>322</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="17">
         <v>492</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="17">
         <v>493</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="17">
         <v>185</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G19" s="17">
         <v>143</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="17">
         <v>268</v>
       </c>
-      <c r="I19" s="22">
+      <c r="I19" s="17">
         <v>380</v>
       </c>
-      <c r="J19" s="22">
+      <c r="J19" s="17">
         <v>325</v>
       </c>
-      <c r="K19" s="22">
+      <c r="K19" s="17">
         <v>382</v>
       </c>
-      <c r="L19" s="22">
+      <c r="L19" s="17">
         <v>148</v>
       </c>
-      <c r="M19" s="22">
+      <c r="M19" s="17">
         <v>328</v>
       </c>
-      <c r="N19" s="22">
+      <c r="N19" s="17">
         <v>449</v>
       </c>
-      <c r="O19" s="22">
+      <c r="O19" s="17">
         <v>238</v>
       </c>
-      <c r="P19" s="22">
+      <c r="P19" s="17">
         <v>180</v>
       </c>
-      <c r="Q19" s="22">
+      <c r="Q19" s="17">
         <v>303</v>
       </c>
-      <c r="R19" s="22">
+      <c r="R19" s="17">
         <v>164</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="17">
+        <v>50</v>
+      </c>
+      <c r="D20" s="17">
+        <v>41</v>
+      </c>
+      <c r="E20" s="17">
+        <v>36</v>
+      </c>
+      <c r="F20" s="17">
+        <v>39</v>
+      </c>
+      <c r="G20" s="17">
+        <v>24</v>
+      </c>
+      <c r="H20" s="17">
+        <v>21</v>
+      </c>
+      <c r="I20" s="17">
+        <v>28</v>
+      </c>
+      <c r="J20" s="17">
+        <v>20</v>
+      </c>
+      <c r="K20" s="17">
+        <v>55</v>
+      </c>
+      <c r="L20" s="17">
+        <v>64</v>
+      </c>
+      <c r="M20" s="17">
+        <v>63</v>
+      </c>
+      <c r="N20" s="17">
+        <v>295</v>
+      </c>
+      <c r="O20" s="17">
+        <v>672</v>
+      </c>
+      <c r="P20" s="17">
+        <v>582</v>
+      </c>
+      <c r="Q20" s="17">
+        <v>2217</v>
+      </c>
+      <c r="R20" s="17">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="22">
-        <v>50</v>
-      </c>
-      <c r="D20" s="22">
-        <v>41</v>
-      </c>
-      <c r="E20" s="22">
-        <v>36</v>
-      </c>
-      <c r="F20" s="22">
-        <v>39</v>
-      </c>
-      <c r="G20" s="22">
-        <v>24</v>
-      </c>
-      <c r="H20" s="22">
-        <v>21</v>
-      </c>
-      <c r="I20" s="22">
-        <v>28</v>
-      </c>
-      <c r="J20" s="22">
-        <v>20</v>
-      </c>
-      <c r="K20" s="22">
-        <v>55</v>
-      </c>
-      <c r="L20" s="22">
-        <v>64</v>
-      </c>
-      <c r="M20" s="22">
-        <v>63</v>
-      </c>
-      <c r="N20" s="22">
-        <v>295</v>
-      </c>
-      <c r="O20" s="22">
-        <v>672</v>
-      </c>
-      <c r="P20" s="22">
-        <v>582</v>
-      </c>
-      <c r="Q20" s="22">
-        <v>2217</v>
-      </c>
-      <c r="R20" s="22">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="21" spans="2:18" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="21">
+      <c r="C21" s="16">
         <v>1533</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="16">
         <v>1534</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="16">
         <v>1289</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="16">
         <v>1232</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="16">
         <v>1017</v>
       </c>
-      <c r="H21" s="21">
+      <c r="H21" s="16">
         <v>1165</v>
       </c>
-      <c r="I21" s="21">
+      <c r="I21" s="16">
         <v>1263</v>
       </c>
-      <c r="J21" s="21">
+      <c r="J21" s="16">
         <v>1482</v>
       </c>
-      <c r="K21" s="21">
+      <c r="K21" s="16">
         <v>1739</v>
       </c>
-      <c r="L21" s="21">
+      <c r="L21" s="16">
         <v>1769</v>
       </c>
-      <c r="M21" s="21">
+      <c r="M21" s="16">
         <v>1765</v>
       </c>
-      <c r="N21" s="21">
+      <c r="N21" s="16">
         <v>2262</v>
       </c>
-      <c r="O21" s="21">
+      <c r="O21" s="16">
         <v>2787</v>
       </c>
-      <c r="P21" s="21">
+      <c r="P21" s="16">
         <v>2501</v>
       </c>
-      <c r="Q21" s="21">
+      <c r="Q21" s="16">
         <v>4241</v>
       </c>
-      <c r="R21" s="21">
+      <c r="R21" s="16">
         <v>2376</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="22">
+        <v>17</v>
+      </c>
+      <c r="C22" s="17">
         <v>568</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="17">
         <v>525</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="17">
         <v>521</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="17">
         <v>564</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="17">
         <v>542</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="17">
         <v>489</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I22" s="17">
         <v>599</v>
       </c>
-      <c r="J22" s="22">
+      <c r="J22" s="17">
         <v>596</v>
       </c>
-      <c r="K22" s="22">
+      <c r="K22" s="17">
         <v>589</v>
       </c>
-      <c r="L22" s="22">
+      <c r="L22" s="17">
         <v>596</v>
       </c>
-      <c r="M22" s="22">
+      <c r="M22" s="17">
         <v>625</v>
       </c>
-      <c r="N22" s="22">
+      <c r="N22" s="17">
         <v>647</v>
       </c>
-      <c r="O22" s="22">
+      <c r="O22" s="17">
         <v>673</v>
       </c>
-      <c r="P22" s="22">
+      <c r="P22" s="17">
         <v>658</v>
       </c>
-      <c r="Q22" s="22">
+      <c r="Q22" s="17">
         <v>661</v>
       </c>
-      <c r="R22" s="22">
+      <c r="R22" s="17">
         <v>744</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="17">
+        <v>111</v>
+      </c>
+      <c r="D23" s="17">
+        <v>81</v>
+      </c>
+      <c r="E23" s="17">
+        <v>112</v>
+      </c>
+      <c r="F23" s="17">
+        <v>76</v>
+      </c>
+      <c r="G23" s="17">
+        <v>73</v>
+      </c>
+      <c r="H23" s="17">
+        <v>89</v>
+      </c>
+      <c r="I23" s="17">
+        <v>96</v>
+      </c>
+      <c r="J23" s="17">
+        <v>110</v>
+      </c>
+      <c r="K23" s="17">
+        <v>111</v>
+      </c>
+      <c r="L23" s="17">
+        <v>119</v>
+      </c>
+      <c r="M23" s="17">
+        <v>112</v>
+      </c>
+      <c r="N23" s="17">
+        <v>134</v>
+      </c>
+      <c r="O23" s="17">
+        <v>108</v>
+      </c>
+      <c r="P23" s="17">
+        <v>119</v>
+      </c>
+      <c r="Q23" s="17">
+        <v>124</v>
+      </c>
+      <c r="R23" s="17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="22">
-        <v>111</v>
-      </c>
-      <c r="D23" s="22">
-        <v>81</v>
-      </c>
-      <c r="E23" s="22">
-        <v>112</v>
-      </c>
-      <c r="F23" s="22">
-        <v>76</v>
-      </c>
-      <c r="G23" s="22">
-        <v>73</v>
-      </c>
-      <c r="H23" s="22">
-        <v>89</v>
-      </c>
-      <c r="I23" s="22">
-        <v>96</v>
-      </c>
-      <c r="J23" s="22">
-        <v>110</v>
-      </c>
-      <c r="K23" s="22">
-        <v>111</v>
-      </c>
-      <c r="L23" s="22">
-        <v>119</v>
-      </c>
-      <c r="M23" s="22">
-        <v>112</v>
-      </c>
-      <c r="N23" s="22">
-        <v>134</v>
-      </c>
-      <c r="O23" s="22">
-        <v>108</v>
-      </c>
-      <c r="P23" s="22">
-        <v>119</v>
-      </c>
-      <c r="Q23" s="22">
-        <v>124</v>
-      </c>
-      <c r="R23" s="22">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="19" t="s">
+      <c r="C24" s="16">
+        <v>213</v>
+      </c>
+      <c r="D24" s="16">
+        <v>250</v>
+      </c>
+      <c r="E24" s="16">
+        <v>266</v>
+      </c>
+      <c r="F24" s="16">
+        <v>233</v>
+      </c>
+      <c r="G24" s="16">
+        <v>211</v>
+      </c>
+      <c r="H24" s="16">
+        <v>225</v>
+      </c>
+      <c r="I24" s="16">
+        <v>211</v>
+      </c>
+      <c r="J24" s="16">
+        <v>211</v>
+      </c>
+      <c r="K24" s="16">
+        <v>228</v>
+      </c>
+      <c r="L24" s="16">
+        <v>256</v>
+      </c>
+      <c r="M24" s="16">
+        <v>260</v>
+      </c>
+      <c r="N24" s="16">
+        <v>270</v>
+      </c>
+      <c r="O24" s="16">
+        <v>296</v>
+      </c>
+      <c r="P24" s="16">
+        <v>247</v>
+      </c>
+      <c r="Q24" s="16">
+        <v>288</v>
+      </c>
+      <c r="R24" s="16">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="21">
-        <v>213</v>
-      </c>
-      <c r="D24" s="21">
-        <v>250</v>
-      </c>
-      <c r="E24" s="21">
-        <v>266</v>
-      </c>
-      <c r="F24" s="21">
-        <v>233</v>
-      </c>
-      <c r="G24" s="21">
-        <v>211</v>
-      </c>
-      <c r="H24" s="21">
-        <v>225</v>
-      </c>
-      <c r="I24" s="21">
-        <v>211</v>
-      </c>
-      <c r="J24" s="21">
-        <v>211</v>
-      </c>
-      <c r="K24" s="21">
-        <v>228</v>
-      </c>
-      <c r="L24" s="21">
-        <v>256</v>
-      </c>
-      <c r="M24" s="21">
-        <v>260</v>
-      </c>
-      <c r="N24" s="21">
-        <v>270</v>
-      </c>
-      <c r="O24" s="21">
-        <v>296</v>
-      </c>
-      <c r="P24" s="21">
-        <v>247</v>
-      </c>
-      <c r="Q24" s="21">
-        <v>288</v>
-      </c>
-      <c r="R24" s="21">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="21">
+      <c r="C25" s="16">
         <v>2704</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="16">
         <v>2851</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="16">
         <v>2375</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="16">
         <v>2272</v>
       </c>
-      <c r="G25" s="21">
+      <c r="G25" s="16">
         <v>2338</v>
       </c>
-      <c r="H25" s="21">
+      <c r="H25" s="16">
         <v>2290</v>
       </c>
-      <c r="I25" s="21">
+      <c r="I25" s="16">
         <v>2443</v>
       </c>
-      <c r="J25" s="21">
+      <c r="J25" s="16">
         <v>2488</v>
       </c>
-      <c r="K25" s="21">
+      <c r="K25" s="16">
         <v>2348</v>
       </c>
-      <c r="L25" s="21">
+      <c r="L25" s="16">
         <v>2364</v>
       </c>
-      <c r="M25" s="21">
+      <c r="M25" s="16">
         <v>2392</v>
       </c>
-      <c r="N25" s="21">
+      <c r="N25" s="16">
         <v>2614</v>
       </c>
-      <c r="O25" s="21">
+      <c r="O25" s="16">
         <v>2599</v>
       </c>
-      <c r="P25" s="21">
+      <c r="P25" s="16">
         <v>2694</v>
       </c>
-      <c r="Q25" s="21">
+      <c r="Q25" s="16">
         <v>3120</v>
       </c>
-      <c r="R25" s="21">
+      <c r="R25" s="16">
         <v>3645</v>
       </c>
     </row>
     <row r="26" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="22">
+        <v>21</v>
+      </c>
+      <c r="C26" s="17">
         <v>236</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="17">
         <v>227</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="17">
         <v>230</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F26" s="17">
         <v>219</v>
       </c>
-      <c r="G26" s="22">
+      <c r="G26" s="17">
         <v>210</v>
       </c>
-      <c r="H26" s="22">
+      <c r="H26" s="17">
         <v>161</v>
       </c>
-      <c r="I26" s="22">
+      <c r="I26" s="17">
         <v>124</v>
       </c>
-      <c r="J26" s="22">
+      <c r="J26" s="17">
         <v>121</v>
       </c>
-      <c r="K26" s="22">
+      <c r="K26" s="17">
         <v>129</v>
       </c>
-      <c r="L26" s="22">
+      <c r="L26" s="17">
         <v>129</v>
       </c>
-      <c r="M26" s="22">
+      <c r="M26" s="17">
         <v>129</v>
       </c>
-      <c r="N26" s="22">
+      <c r="N26" s="17">
         <v>150</v>
       </c>
-      <c r="O26" s="22">
+      <c r="O26" s="17">
         <v>158</v>
       </c>
-      <c r="P26" s="22">
+      <c r="P26" s="17">
         <v>131</v>
       </c>
-      <c r="Q26" s="22">
+      <c r="Q26" s="17">
         <v>167</v>
       </c>
-      <c r="R26" s="22">
+      <c r="R26" s="17">
         <v>184</v>
       </c>
     </row>
     <row r="27" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="22">
+        <v>22</v>
+      </c>
+      <c r="C27" s="17">
         <v>395</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="17">
         <v>454</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="17">
         <v>377</v>
       </c>
-      <c r="F27" s="22">
+      <c r="F27" s="17">
         <v>367</v>
       </c>
-      <c r="G27" s="22">
+      <c r="G27" s="17">
         <v>335</v>
       </c>
-      <c r="H27" s="22">
+      <c r="H27" s="17">
         <v>295</v>
       </c>
-      <c r="I27" s="22">
+      <c r="I27" s="17">
         <v>240</v>
       </c>
-      <c r="J27" s="22">
+      <c r="J27" s="17">
         <v>209</v>
       </c>
-      <c r="K27" s="22">
+      <c r="K27" s="17">
         <v>243</v>
       </c>
-      <c r="L27" s="22">
+      <c r="L27" s="17">
         <v>254</v>
       </c>
-      <c r="M27" s="22">
+      <c r="M27" s="17">
         <v>259</v>
       </c>
-      <c r="N27" s="22">
+      <c r="N27" s="17">
         <v>303</v>
       </c>
-      <c r="O27" s="22">
+      <c r="O27" s="17">
         <v>238</v>
       </c>
-      <c r="P27" s="22">
+      <c r="P27" s="17">
         <v>233</v>
       </c>
-      <c r="Q27" s="22">
+      <c r="Q27" s="17">
         <v>209</v>
       </c>
-      <c r="R27" s="22">
+      <c r="R27" s="17">
         <v>194</v>
       </c>
     </row>
     <row r="28" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="22">
+        <v>23</v>
+      </c>
+      <c r="C28" s="17">
         <v>52</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28" s="17">
         <v>44</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E28" s="17">
         <v>33</v>
       </c>
-      <c r="F28" s="22">
+      <c r="F28" s="17">
         <v>38</v>
       </c>
-      <c r="G28" s="22">
+      <c r="G28" s="17">
         <v>34</v>
       </c>
-      <c r="H28" s="22">
+      <c r="H28" s="17">
         <v>41</v>
       </c>
-      <c r="I28" s="22">
+      <c r="I28" s="17">
         <v>44</v>
       </c>
-      <c r="J28" s="22">
+      <c r="J28" s="17">
         <v>64</v>
       </c>
-      <c r="K28" s="22">
+      <c r="K28" s="17">
         <v>61</v>
       </c>
-      <c r="L28" s="22">
+      <c r="L28" s="17">
         <v>63</v>
       </c>
-      <c r="M28" s="22">
+      <c r="M28" s="17">
         <v>65</v>
       </c>
-      <c r="N28" s="22">
+      <c r="N28" s="17">
         <v>96</v>
       </c>
-      <c r="O28" s="22">
+      <c r="O28" s="17">
         <v>103</v>
       </c>
-      <c r="P28" s="22">
+      <c r="P28" s="17">
         <v>73</v>
       </c>
-      <c r="Q28" s="22">
+      <c r="Q28" s="17">
         <v>157</v>
       </c>
-      <c r="R28" s="22">
+      <c r="R28" s="17">
         <v>117</v>
       </c>
     </row>
     <row r="29" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="22">
+        <v>24</v>
+      </c>
+      <c r="C29" s="17">
         <v>516</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="17">
         <v>251</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="17">
         <v>286</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F29" s="17">
         <v>306</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="17">
         <v>361</v>
       </c>
-      <c r="H29" s="22">
+      <c r="H29" s="17">
         <v>392</v>
       </c>
-      <c r="I29" s="22">
+      <c r="I29" s="17">
         <v>434</v>
       </c>
-      <c r="J29" s="22">
+      <c r="J29" s="17">
         <v>273</v>
       </c>
-      <c r="K29" s="22">
+      <c r="K29" s="17">
         <v>326</v>
       </c>
-      <c r="L29" s="22">
+      <c r="L29" s="17">
         <v>317</v>
       </c>
-      <c r="M29" s="22">
+      <c r="M29" s="17">
         <v>313</v>
       </c>
-      <c r="N29" s="22">
+      <c r="N29" s="17">
         <v>430</v>
       </c>
-      <c r="O29" s="22">
+      <c r="O29" s="17">
         <v>403</v>
       </c>
-      <c r="P29" s="22">
+      <c r="P29" s="17">
         <v>389</v>
       </c>
-      <c r="Q29" s="22">
+      <c r="Q29" s="17">
         <v>465</v>
       </c>
-      <c r="R29" s="22">
+      <c r="R29" s="17">
         <v>477</v>
       </c>
     </row>
     <row r="30" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="22">
+        <v>25</v>
+      </c>
+      <c r="C30" s="17">
         <v>348</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="17">
         <v>386</v>
       </c>
-      <c r="E30" s="22">
+      <c r="E30" s="17">
         <v>362</v>
       </c>
-      <c r="F30" s="22">
+      <c r="F30" s="17">
         <v>303</v>
       </c>
-      <c r="G30" s="22">
+      <c r="G30" s="17">
         <v>323</v>
       </c>
-      <c r="H30" s="22">
+      <c r="H30" s="17">
         <v>245</v>
       </c>
-      <c r="I30" s="22">
+      <c r="I30" s="17">
         <v>255</v>
       </c>
-      <c r="J30" s="22">
+      <c r="J30" s="17">
         <v>227</v>
       </c>
-      <c r="K30" s="22">
+      <c r="K30" s="17">
         <v>227</v>
       </c>
-      <c r="L30" s="22">
+      <c r="L30" s="17">
         <v>262</v>
       </c>
-      <c r="M30" s="22">
+      <c r="M30" s="17">
         <v>221</v>
       </c>
-      <c r="N30" s="22">
+      <c r="N30" s="17">
         <v>255</v>
       </c>
-      <c r="O30" s="22">
+      <c r="O30" s="17">
         <v>260</v>
       </c>
-      <c r="P30" s="22">
+      <c r="P30" s="17">
         <v>243</v>
       </c>
-      <c r="Q30" s="22">
+      <c r="Q30" s="17">
         <v>308</v>
       </c>
-      <c r="R30" s="22">
+      <c r="R30" s="17">
         <v>336</v>
       </c>
     </row>
     <row r="31" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="22">
+        <v>26</v>
+      </c>
+      <c r="C31" s="17">
         <v>87</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="17">
         <v>76</v>
       </c>
-      <c r="E31" s="22">
+      <c r="E31" s="17">
         <v>46</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F31" s="17">
         <v>52</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G31" s="17">
         <v>67</v>
       </c>
-      <c r="H31" s="22">
+      <c r="H31" s="17">
         <v>33</v>
       </c>
-      <c r="I31" s="22">
+      <c r="I31" s="17">
         <v>47</v>
       </c>
-      <c r="J31" s="22">
+      <c r="J31" s="17">
         <v>49</v>
       </c>
-      <c r="K31" s="22">
+      <c r="K31" s="17">
         <v>40</v>
       </c>
-      <c r="L31" s="22">
+      <c r="L31" s="17">
         <v>61</v>
       </c>
-      <c r="M31" s="22">
+      <c r="M31" s="17">
         <v>66</v>
       </c>
-      <c r="N31" s="22">
+      <c r="N31" s="17">
         <v>77</v>
       </c>
-      <c r="O31" s="22">
+      <c r="O31" s="17">
         <v>60</v>
       </c>
-      <c r="P31" s="22">
+      <c r="P31" s="17">
         <v>57</v>
       </c>
-      <c r="Q31" s="22">
+      <c r="Q31" s="17">
         <v>77</v>
       </c>
-      <c r="R31" s="22">
+      <c r="R31" s="17">
         <v>120</v>
       </c>
     </row>
     <row r="32" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="22">
+        <v>27</v>
+      </c>
+      <c r="C32" s="17">
         <v>171</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D32" s="17">
         <v>183</v>
       </c>
-      <c r="E32" s="22">
+      <c r="E32" s="17">
         <v>210</v>
       </c>
-      <c r="F32" s="22">
+      <c r="F32" s="17">
         <v>208</v>
       </c>
-      <c r="G32" s="22">
+      <c r="G32" s="17">
         <v>225</v>
       </c>
-      <c r="H32" s="22">
+      <c r="H32" s="17">
         <v>219</v>
       </c>
-      <c r="I32" s="22">
+      <c r="I32" s="17">
         <v>219</v>
       </c>
-      <c r="J32" s="22">
+      <c r="J32" s="17">
         <v>208</v>
       </c>
-      <c r="K32" s="22">
+      <c r="K32" s="17">
         <v>247</v>
       </c>
-      <c r="L32" s="22">
+      <c r="L32" s="17">
         <v>300</v>
       </c>
-      <c r="M32" s="22">
+      <c r="M32" s="17">
         <v>398</v>
       </c>
-      <c r="N32" s="22">
+      <c r="N32" s="17">
         <v>368</v>
       </c>
-      <c r="O32" s="22">
+      <c r="O32" s="17">
         <v>444</v>
       </c>
-      <c r="P32" s="22">
+      <c r="P32" s="17">
         <v>664</v>
       </c>
-      <c r="Q32" s="22">
+      <c r="Q32" s="17">
         <v>857</v>
       </c>
-      <c r="R32" s="22">
+      <c r="R32" s="17">
         <v>1414</v>
       </c>
     </row>
     <row r="33" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="22">
+        <v>28</v>
+      </c>
+      <c r="C33" s="17">
         <v>137</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="17">
         <v>160</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E33" s="17">
         <v>158</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F33" s="17">
         <v>110</v>
       </c>
-      <c r="G33" s="22">
+      <c r="G33" s="17">
         <v>227</v>
       </c>
-      <c r="H33" s="22">
+      <c r="H33" s="17">
         <v>280</v>
       </c>
-      <c r="I33" s="22">
+      <c r="I33" s="17">
         <v>419</v>
       </c>
-      <c r="J33" s="22">
+      <c r="J33" s="17">
         <v>667</v>
       </c>
-      <c r="K33" s="22">
+      <c r="K33" s="17">
         <v>387</v>
       </c>
-      <c r="L33" s="22">
+      <c r="L33" s="17">
         <v>277</v>
       </c>
-      <c r="M33" s="22">
+      <c r="M33" s="17">
         <v>266</v>
       </c>
-      <c r="N33" s="22">
+      <c r="N33" s="17">
         <v>265</v>
       </c>
-      <c r="O33" s="22">
+      <c r="O33" s="17">
         <v>259</v>
       </c>
-      <c r="P33" s="22">
+      <c r="P33" s="17">
         <v>290</v>
       </c>
-      <c r="Q33" s="22">
+      <c r="Q33" s="17">
         <v>224</v>
       </c>
-      <c r="R33" s="22">
+      <c r="R33" s="17">
         <v>199</v>
       </c>
     </row>
     <row r="34" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="22">
+        <v>29</v>
+      </c>
+      <c r="C34" s="17">
         <v>1</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="17">
         <v>2</v>
       </c>
-      <c r="E34" s="22">
+      <c r="E34" s="17">
         <v>1</v>
       </c>
-      <c r="F34" s="22">
+      <c r="F34" s="17">
         <v>0</v>
       </c>
-      <c r="G34" s="22">
+      <c r="G34" s="17">
         <v>1</v>
       </c>
-      <c r="H34" s="22">
+      <c r="H34" s="17">
         <v>2</v>
       </c>
-      <c r="I34" s="22">
+      <c r="I34" s="17">
         <v>3</v>
       </c>
-      <c r="J34" s="22">
+      <c r="J34" s="17">
         <v>2</v>
       </c>
-      <c r="K34" s="22">
+      <c r="K34" s="17">
         <v>1</v>
       </c>
-      <c r="L34" s="22">
+      <c r="L34" s="17">
         <v>0</v>
       </c>
-      <c r="M34" s="22">
+      <c r="M34" s="17">
         <v>1</v>
       </c>
-      <c r="N34" s="22">
+      <c r="N34" s="17">
         <v>0</v>
       </c>
-      <c r="O34" s="22">
+      <c r="O34" s="17">
         <v>2</v>
       </c>
-      <c r="P34" s="22">
+      <c r="P34" s="17">
         <v>1</v>
       </c>
-      <c r="Q34" s="22">
+      <c r="Q34" s="17">
         <v>3</v>
       </c>
-      <c r="R34" s="22">
+      <c r="R34" s="17">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="22">
+        <v>30</v>
+      </c>
+      <c r="C35" s="17">
         <v>222</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="17">
         <v>246</v>
       </c>
-      <c r="E35" s="22">
+      <c r="E35" s="17">
         <v>222</v>
       </c>
-      <c r="F35" s="22">
+      <c r="F35" s="17">
         <v>147</v>
       </c>
-      <c r="G35" s="22">
+      <c r="G35" s="17">
         <v>184</v>
       </c>
-      <c r="H35" s="22">
+      <c r="H35" s="17">
         <v>152</v>
       </c>
-      <c r="I35" s="22">
+      <c r="I35" s="17">
         <v>144</v>
       </c>
-      <c r="J35" s="22">
+      <c r="J35" s="17">
         <v>133</v>
       </c>
-      <c r="K35" s="22">
+      <c r="K35" s="17">
         <v>150</v>
       </c>
-      <c r="L35" s="22">
+      <c r="L35" s="17">
         <v>107</v>
       </c>
-      <c r="M35" s="22">
+      <c r="M35" s="17">
         <v>112</v>
       </c>
-      <c r="N35" s="22">
+      <c r="N35" s="17">
         <v>108</v>
       </c>
-      <c r="O35" s="22">
+      <c r="O35" s="17">
         <v>171</v>
       </c>
-      <c r="P35" s="22">
+      <c r="P35" s="17">
         <v>127</v>
       </c>
-      <c r="Q35" s="22">
+      <c r="Q35" s="17">
         <v>137</v>
       </c>
-      <c r="R35" s="22">
+      <c r="R35" s="17">
         <v>171</v>
       </c>
     </row>
     <row r="36" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="17">
+        <v>150</v>
+      </c>
+      <c r="D36" s="17">
+        <v>171</v>
+      </c>
+      <c r="E36" s="17">
+        <v>136</v>
+      </c>
+      <c r="F36" s="17">
+        <v>99</v>
+      </c>
+      <c r="G36" s="17">
+        <v>125</v>
+      </c>
+      <c r="H36" s="17">
+        <v>125</v>
+      </c>
+      <c r="I36" s="17">
+        <v>99</v>
+      </c>
+      <c r="J36" s="17">
+        <v>117</v>
+      </c>
+      <c r="K36" s="17">
+        <v>113</v>
+      </c>
+      <c r="L36" s="17">
+        <v>83</v>
+      </c>
+      <c r="M36" s="17">
+        <v>80</v>
+      </c>
+      <c r="N36" s="17">
+        <v>70</v>
+      </c>
+      <c r="O36" s="17">
+        <v>138</v>
+      </c>
+      <c r="P36" s="17">
+        <v>104</v>
+      </c>
+      <c r="Q36" s="17">
+        <v>115</v>
+      </c>
+      <c r="R36" s="17">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="22">
-        <v>150</v>
-      </c>
-      <c r="D36" s="22">
-        <v>171</v>
-      </c>
-      <c r="E36" s="22">
-        <v>136</v>
-      </c>
-      <c r="F36" s="22">
-        <v>99</v>
-      </c>
-      <c r="G36" s="22">
-        <v>125</v>
-      </c>
-      <c r="H36" s="22">
-        <v>125</v>
-      </c>
-      <c r="I36" s="22">
-        <v>99</v>
-      </c>
-      <c r="J36" s="22">
-        <v>117</v>
-      </c>
-      <c r="K36" s="22">
-        <v>113</v>
-      </c>
-      <c r="L36" s="22">
-        <v>83</v>
-      </c>
-      <c r="M36" s="22">
-        <v>80</v>
-      </c>
-      <c r="N36" s="22">
-        <v>70</v>
-      </c>
-      <c r="O36" s="22">
-        <v>138</v>
-      </c>
-      <c r="P36" s="22">
-        <v>104</v>
-      </c>
-      <c r="Q36" s="22">
-        <v>115</v>
-      </c>
-      <c r="R36" s="22">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="37" spans="2:18" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="24">
+      <c r="C37" s="19">
         <v>10886</v>
       </c>
-      <c r="D37" s="24">
+      <c r="D37" s="19">
         <v>11441</v>
       </c>
-      <c r="E37" s="24">
+      <c r="E37" s="19">
         <v>9251</v>
       </c>
-      <c r="F37" s="24">
+      <c r="F37" s="19">
         <v>7704</v>
       </c>
-      <c r="G37" s="24">
+      <c r="G37" s="19">
         <v>7223</v>
       </c>
-      <c r="H37" s="24">
+      <c r="H37" s="19">
         <v>7363</v>
       </c>
-      <c r="I37" s="24">
+      <c r="I37" s="19">
         <v>7995</v>
       </c>
-      <c r="J37" s="24">
+      <c r="J37" s="19">
         <v>8526</v>
       </c>
-      <c r="K37" s="24">
+      <c r="K37" s="19">
         <v>8216</v>
       </c>
-      <c r="L37" s="24">
+      <c r="L37" s="19">
         <v>7722</v>
       </c>
-      <c r="M37" s="24">
+      <c r="M37" s="19">
         <v>7988</v>
       </c>
-      <c r="N37" s="24">
+      <c r="N37" s="19">
         <v>8519</v>
       </c>
-      <c r="O37" s="24">
+      <c r="O37" s="19">
         <v>8785</v>
       </c>
-      <c r="P37" s="24">
+      <c r="P37" s="19">
         <v>8470</v>
       </c>
-      <c r="Q37" s="24">
+      <c r="Q37" s="19">
         <v>10932</v>
       </c>
-      <c r="R37" s="24">
+      <c r="R37" s="19">
         <v>8878</v>
       </c>
     </row>
@@ -2920,7 +2940,7 @@
     </row>
     <row r="39" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -2940,28 +2960,28 @@
       <c r="R39" s="3"/>
     </row>
     <row r="40" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="10"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
+      <c r="B40" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="3"/>
     </row>
     <row r="41" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="10" t="s">
-        <v>35</v>
-      </c>
+      <c r="B41" s="10"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -2980,7 +3000,9 @@
       <c r="R41" s="2"/>
     </row>
     <row r="42" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="10"/>
+      <c r="B42" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2999,9 +3021,7 @@
       <c r="R42" s="2"/>
     </row>
     <row r="43" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="10" t="s">
-        <v>36</v>
-      </c>
+      <c r="B43" s="10"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -3021,7 +3041,7 @@
     </row>
     <row r="44" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -3042,7 +3062,7 @@
     </row>
     <row r="45" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -3062,8 +3082,8 @@
       <c r="R45" s="2"/>
     </row>
     <row r="46" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="12" t="s">
-        <v>39</v>
+      <c r="B46" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -3082,6 +3102,27 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
+    <row r="47" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B6:B8"/>
@@ -3089,7 +3130,7 @@
     <mergeCell ref="C8:R8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B46" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B47" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ bd93a0977d86ae74dc32af861647b2c21aeb6ed5 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_2-3-4.xlsx
+++ b/assets/excel/2021_2-3-4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E159341-5232-49C3-B2AC-874D2705D36C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD5C95D-3B46-40DF-BD9E-9B49A6F8A5B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{0C07CBDE-D804-47FE-A309-854275EC75AA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
   </si>
@@ -34,6 +34,154 @@
   </si>
   <si>
     <t>Tabelle 2.3.4: Einbürgerungen in Niedersachsen nach ausgewählten Staatsangehörigkeiten</t>
+  </si>
+  <si>
+    <t>Einbürgerungen</t>
+  </si>
+  <si>
+    <t>Anzahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Europa insgesamt            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Griechenland              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Italien                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kosovo                    </t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Polen                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Rumänien                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Russische Föderation      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Türkei                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ukraine                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EU Staaten                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afrika insgesamt            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Tunesien                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amerika insgesamt           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asien insgesamt             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Afganistan                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Libanon                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Indien                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Irak                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Iran, Islamische Republik </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Pakistan                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Syrien, Arabische Republik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Vietnam                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australien und Ozeanien     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonstige Ziele              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  staatenlos                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insgesamt                   </t>
+  </si>
+  <si>
+    <t>Quelle: Einbürgerungsstatistik</t>
+  </si>
+  <si>
+    <t>Niedersächsisches Ministerium für Soziales, Gesundheit und Gleichstellung (Hrsg.),</t>
+  </si>
+  <si>
+    <t>© Landesamt für Statistik Niedersachsen, Hannover 2021,                                                                          </t>
+  </si>
+  <si>
+    <t>Vervielfältigung und Verbreitung, auch auszugsweise, mit Quellenangabe gestattet.</t>
+  </si>
+  <si>
+    <t>https://www.integrationsmonitoring.niedersachsen.de</t>
+  </si>
+  <si>
+    <t>1) Aufgeführt sind die 20 häufigsten Staatsangehörigkeiten der Ausländerinnen und Ausländer im Jahr 2020 in Niedersachsen.</t>
+  </si>
+  <si>
+    <t>2) 2005 Serbien und Montenegro , 2006-2008 Serbien und Kosovo, ab 2009 Serbien</t>
+  </si>
+  <si>
+    <t>3) einschließlich Britisch abhängiger Gebiete</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  Serbien </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="NDSFrutiger 45 Light"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="NDSFrutiger 45 Light"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  Vereinigtes Königreich GB, Nordirland</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="NDSFrutiger 45 Light"/>
+      </rPr>
+      <t>3)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -46,144 +194,8 @@
         <sz val="6"/>
         <rFont val="NDSFrutiger 45 Light"/>
       </rPr>
-      <t>1,2)</t>
+      <t>2,3)</t>
     </r>
-  </si>
-  <si>
-    <t>Einbürgerungen</t>
-  </si>
-  <si>
-    <t>Anzahl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Europa insgesamt            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Griechenland              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Italien                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Kosovo                    </t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Polen                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Rumänien                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Russische Föderation      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Türkei                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Ukraine                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EU Staaten                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afrika insgesamt            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Tunesien                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amerika insgesamt           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asien insgesamt             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Afganistan                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Libanon                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Indien                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Irak                      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Iran, Islamische Republik </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Pakistan                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Syrien, Arabische Republik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Vietnam                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Australien und Ozeanien     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sonstige Ziele              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  staatenlos                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insgesamt                   </t>
-  </si>
-  <si>
-    <t>1) 2005 Serbien und Montenegro , 2006-2008 Serbien und Kosovo, ab 2009 Serbien</t>
-  </si>
-  <si>
-    <t>Quelle: Einbürgerungsstatistik</t>
-  </si>
-  <si>
-    <t>Niedersächsisches Ministerium für Soziales, Gesundheit und Gleichstellung (Hrsg.),</t>
-  </si>
-  <si>
-    <t>© Landesamt für Statistik Niedersachsen, Hannover 2021,                                                                          </t>
-  </si>
-  <si>
-    <t>Vervielfältigung und Verbreitung, auch auszugsweise, mit Quellenangabe gestattet.</t>
-  </si>
-  <si>
-    <t>https://www.integrationsmonitoring.niedersachsen.de</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">  Serbien </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="6"/>
-        <color indexed="8"/>
-        <rFont val="NDSFrutiger 45 Light"/>
-      </rPr>
-      <t>1)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">  Vereinigtes Königreich GB, Nordirland</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="6"/>
-        <color theme="1"/>
-        <rFont val="NDSFrutiger 45 Light"/>
-      </rPr>
-      <t>2)</t>
-    </r>
-  </si>
-  <si>
-    <t>2) einschließlich Brittisch abhängiger Gebiete</t>
   </si>
 </sst>
 </file>
@@ -563,7 +575,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -737,6 +749,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -784,7 +805,7 @@
     <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyAlignment="1">
@@ -852,6 +873,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="15" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1211,10 +1235,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7E64D10-9C9A-44E2-8806-D26C8D26226A}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="B1:R47"/>
+  <dimension ref="B1:R48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,10 +1313,10 @@
     </row>
     <row r="6" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>3</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>4</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -1364,7 +1388,7 @@
     <row r="8" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
       <c r="C8" s="23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -1437,7 +1461,7 @@
     </row>
     <row r="10" spans="2:18" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="16">
         <v>7178</v>
@@ -1490,7 +1514,7 @@
     </row>
     <row r="11" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="17">
         <v>71</v>
@@ -1543,7 +1567,7 @@
     </row>
     <row r="12" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="17">
         <v>71</v>
@@ -1596,19 +1620,19 @@
     </row>
     <row r="13" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>10</v>
-      </c>
       <c r="D13" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G13" s="17">
         <v>34</v>
@@ -1649,7 +1673,7 @@
     </row>
     <row r="14" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="17">
         <v>914</v>
@@ -1702,7 +1726,7 @@
     </row>
     <row r="15" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="17">
         <v>72</v>
@@ -1755,7 +1779,7 @@
     </row>
     <row r="16" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="17">
         <v>496</v>
@@ -1808,7 +1832,7 @@
     </row>
     <row r="17" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17" s="17">
         <v>1630</v>
@@ -1861,7 +1885,7 @@
     </row>
     <row r="18" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="17">
         <v>2897</v>
@@ -1914,7 +1938,7 @@
     </row>
     <row r="19" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="17">
         <v>322</v>
@@ -1967,7 +1991,7 @@
     </row>
     <row r="20" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" s="17">
         <v>50</v>
@@ -2020,7 +2044,7 @@
     </row>
     <row r="21" spans="2:18" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="16">
         <v>1533</v>
@@ -2073,7 +2097,7 @@
     </row>
     <row r="22" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="17">
         <v>568</v>
@@ -2126,7 +2150,7 @@
     </row>
     <row r="23" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="17">
         <v>111</v>
@@ -2179,7 +2203,7 @@
     </row>
     <row r="24" spans="2:18" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="16">
         <v>213</v>
@@ -2232,7 +2256,7 @@
     </row>
     <row r="25" spans="2:18" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="16">
         <v>2704</v>
@@ -2285,7 +2309,7 @@
     </row>
     <row r="26" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="17">
         <v>236</v>
@@ -2338,7 +2362,7 @@
     </row>
     <row r="27" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="17">
         <v>395</v>
@@ -2391,7 +2415,7 @@
     </row>
     <row r="28" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="17">
         <v>52</v>
@@ -2444,7 +2468,7 @@
     </row>
     <row r="29" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="17">
         <v>516</v>
@@ -2497,7 +2521,7 @@
     </row>
     <row r="30" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" s="17">
         <v>348</v>
@@ -2550,7 +2574,7 @@
     </row>
     <row r="31" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="17">
         <v>87</v>
@@ -2603,7 +2627,7 @@
     </row>
     <row r="32" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" s="17">
         <v>171</v>
@@ -2656,7 +2680,7 @@
     </row>
     <row r="33" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C33" s="17">
         <v>137</v>
@@ -2709,7 +2733,7 @@
     </row>
     <row r="34" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C34" s="17">
         <v>1</v>
@@ -2762,7 +2786,7 @@
     </row>
     <row r="35" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C35" s="17">
         <v>222</v>
@@ -2815,7 +2839,7 @@
     </row>
     <row r="36" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C36" s="17">
         <v>150</v>
@@ -2868,7 +2892,7 @@
     </row>
     <row r="37" spans="2:18" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37" s="19">
         <v>10886</v>
@@ -2939,8 +2963,8 @@
       <c r="R38" s="3"/>
     </row>
     <row r="39" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="10" t="s">
-        <v>33</v>
+      <c r="B39" s="25" t="s">
+        <v>37</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -2961,7 +2985,7 @@
     </row>
     <row r="40" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -2981,28 +3005,28 @@
       <c r="R40" s="3"/>
     </row>
     <row r="41" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="10"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
-      <c r="Q41" s="2"/>
-      <c r="R41" s="2"/>
+      <c r="B41" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="3"/>
     </row>
     <row r="42" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="10" t="s">
-        <v>34</v>
-      </c>
+      <c r="B42" s="10"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -3021,7 +3045,9 @@
       <c r="R42" s="2"/>
     </row>
     <row r="43" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="10"/>
+      <c r="B43" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -3040,9 +3066,7 @@
       <c r="R43" s="2"/>
     </row>
     <row r="44" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="10" t="s">
-        <v>35</v>
-      </c>
+      <c r="B44" s="10"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -3062,7 +3086,7 @@
     </row>
     <row r="45" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -3083,7 +3107,7 @@
     </row>
     <row r="46" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -3103,8 +3127,8 @@
       <c r="R46" s="2"/>
     </row>
     <row r="47" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="12" t="s">
-        <v>38</v>
+      <c r="B47" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -3123,6 +3147,27 @@
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
     </row>
+    <row r="48" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B6:B8"/>
@@ -3130,7 +3175,7 @@
     <mergeCell ref="C8:R8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B47" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B48" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>